<commit_message>
Tableau de case avec ids
</commit_message>
<xml_diff>
--- a/src/images/Map.xlsx
+++ b/src/images/Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Titouan\Documents\git\Projet-Comm_M1ICE\src\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4410DE6E-000C-41BA-A376-205D7472931A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7D74B49-E999-48B1-B32B-CE1A0EAA67A2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7D58ACB1-F20F-4645-9C2B-F8E869CAF51A}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ville</t>
   </si>
@@ -43,6 +44,9 @@
   </si>
   <si>
     <t>Camp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -453,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0995F3E-F952-4EF7-A5E6-9C4F4860FE13}">
-  <dimension ref="A1:AK24"/>
+  <dimension ref="A1:AK28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH13" sqref="AH13"/>
+      <selection activeCell="AB28" sqref="AB28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,7 +898,7 @@
       <c r="S12" s="5"/>
       <c r="T12" s="1"/>
       <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
+      <c r="V12" s="6"/>
       <c r="W12" s="4"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
@@ -930,7 +934,7 @@
       <c r="R13" s="5"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
+      <c r="U13" s="4"/>
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="6"/>
@@ -1376,6 +1380,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AA28" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>